<commit_message>
updated summary of the results
</commit_message>
<xml_diff>
--- a/3D_Imaging/CellCycleMaps/Dataset_merged/Results_summary.xlsx
+++ b/3D_Imaging/CellCycleMaps/Dataset_merged/Results_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saeedalahmari/Downloads/PMO_MeasuringFitnessperClone/3D_Imaging/CellCycleMaps/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saeedalahmari/Downloads/PMO_MeasuringFitnessperClone/3D_Imaging/CellCycleMaps/Dataset_merged/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F3B3F4-0C8E-5B4D-B1DD-7BDAF5E06A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4891B58-0002-2841-A70D-DA870C123542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33400" yWindow="2240" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{04CE307E-20E2-444B-BA0B-F2525E8E21F9}"/>
+    <workbookView xWindow="43060" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{04CE307E-20E2-444B-BA0B-F2525E8E21F9}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -133,6 +130,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,96 +470,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BC4EFB-84A5-F647-86CA-4F5FE6771BB9}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="10.83203125" style="4"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.63460000000000005</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="2"/>
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3">
-        <v>0.74919999999999998</v>
+      <c r="E3" s="2">
+        <v>0.85750000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.75280000000000002</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="2"/>
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3">
-        <v>0.82450000000000001</v>
+      <c r="E4" s="2">
+        <v>0.83220000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.67459999999999998</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="2"/>
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="3">
-        <v>0.77100000000000002</v>
+      <c r="E5" s="2">
+        <v>0.86739999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.65990000000000004</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="B6" s="2"/>
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3">
-        <v>0.74690000000000001</v>
+      <c r="E6" s="2">
+        <v>0.83189999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -575,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76655F87-CC55-3F45-8E1F-A7124DABE50B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,76 +580,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="2"/>
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3">
-        <v>0.43030000000000002</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="2"/>
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3">
-        <v>0.57740000000000002</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="2"/>
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="3">
-        <v>0.71079999999999999</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="D6" s="4" t="s">
+      <c r="B6" s="2"/>
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3">
-        <v>0.5222</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
added results for single channel CNN model train on merged data
</commit_message>
<xml_diff>
--- a/3D_Imaging/CellCycleMaps/Dataset_merged/Results_summary.xlsx
+++ b/3D_Imaging/CellCycleMaps/Dataset_merged/Results_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saeedalahmari/Downloads/PMO_MeasuringFitnessperClone/3D_Imaging/CellCycleMaps/Dataset_merged/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4891B58-0002-2841-A70D-DA870C123542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276A42BF-0187-354A-A556-2E2510D05C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43060" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{04CE307E-20E2-444B-BA0B-F2525E8E21F9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{04CE307E-20E2-444B-BA0B-F2525E8E21F9}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +510,9 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>0.71199999999999997</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
@@ -522,7 +524,9 @@
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>0.69779999999999998</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
@@ -534,7 +538,9 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>0.81920000000000004</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
@@ -546,7 +552,9 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>0.84809999999999997</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>